<commit_message>
First transient ERFs with new method
</commit_message>
<xml_diff>
--- a/Processed_data/Data_overview.xlsx
+++ b/Processed_data/Data_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitetetitromso-my.sharepoint.com/personal/hfr003_uit_no/Documents/Papers/ForcingCMIP6/CMIP6-forcing/Processed_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{29E502C2-3395-4642-80FE-6AD2BE6C48FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F95D45C-C12A-1640-AEE0-04A91ED7292B}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{29E502C2-3395-4642-80FE-6AD2BE6C48FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB826BD4-9491-9840-B24F-1F12A5DFEF96}"/>
   <bookViews>
     <workbookView xWindow="13960" yWindow="980" windowWidth="32980" windowHeight="22360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -270,9 +270,6 @@
     <t>EC-Earth3</t>
   </si>
   <si>
-    <t>nan</t>
-  </si>
-  <si>
     <t>256 x 1024 (T255L91)</t>
   </si>
   <si>
@@ -687,9 +684,6 @@
     <t>2 members p1 and p2</t>
   </si>
   <si>
-    <t>many members!</t>
-  </si>
-  <si>
     <t>see notes. Data request sent</t>
   </si>
   <si>
@@ -739,6 +733,12 @@
   </si>
   <si>
     <t>some</t>
+  </si>
+  <si>
+    <t>many members! conflicting values for variable 'lat_bnds' on objects to be combined. You can skip this check by specifying compat='override'.</t>
+  </si>
+  <si>
+    <t>longitude error if loading all members, resulting in nan values</t>
   </si>
 </sst>
 </file>
@@ -1219,7 +1219,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C31" sqref="C31"/>
+      <selection pane="topRight" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1774,44 +1774,44 @@
         <v>59</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>198</v>
-      </c>
       <c r="D23" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="G23" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>198</v>
-      </c>
       <c r="I23" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="N23" s="3"/>
+        <v>196</v>
+      </c>
+      <c r="N23" s="8"/>
       <c r="O23" t="s">
         <v>60</v>
       </c>
       <c r="P23" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Q23" t="s">
         <v>33</v>
@@ -1825,10 +1825,10 @@
         <v>61</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1837,19 +1837,19 @@
         <v>0</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O24" t="s">
         <v>62</v>
@@ -1869,10 +1869,10 @@
         <v>64</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1881,25 +1881,25 @@
         <v>0</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>65</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O25" t="s">
         <v>60</v>
@@ -2070,7 +2070,7 @@
         <v>76</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31">
@@ -2079,30 +2079,30 @@
       <c r="E31">
         <v>0</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="F31" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
       <c r="O31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q31" t="s">
         <v>33</v>
       </c>
       <c r="R31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>43</v>
@@ -2132,12 +2132,12 @@
         <v>0</v>
       </c>
       <c r="O32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2155,7 +2155,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="O33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q33" t="s">
         <v>33</v>
@@ -2163,10 +2163,10 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2191,15 +2191,15 @@
         <v>0</v>
       </c>
       <c r="O34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>48</v>
@@ -2226,7 +2226,7 @@
         <v>48</v>
       </c>
       <c r="O35" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q35" t="s">
         <v>33</v>
@@ -2234,7 +2234,7 @@
     </row>
     <row r="36" spans="1:17">
       <c r="A36" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="3" t="s">
@@ -2255,7 +2255,7 @@
       <c r="J36" s="8"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q36" t="s">
         <v>33</v>
@@ -2263,14 +2263,14 @@
     </row>
     <row r="37" spans="1:17">
       <c r="A37" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="D37">
         <v>0</v>
       </c>
@@ -2278,19 +2278,19 @@
         <v>0</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I37">
         <v>0</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q37" t="s">
         <v>33</v>
@@ -2298,7 +2298,7 @@
     </row>
     <row r="38" spans="1:17">
       <c r="A38" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -2321,7 +2321,7 @@
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
       <c r="O38" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>32</v>
@@ -2332,7 +2332,7 @@
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -2354,7 +2354,7 @@
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
       <c r="O39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P39" s="1" t="s">
         <v>32</v>
@@ -2365,7 +2365,7 @@
     </row>
     <row r="40" spans="1:17">
       <c r="A40" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="10" t="s">
@@ -2392,7 +2392,7 @@
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
       <c r="O40" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P40" s="1" t="s">
         <v>32</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41">
@@ -2429,12 +2429,12 @@
         <v>0</v>
       </c>
       <c r="O41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:17">
       <c r="A42" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>43</v>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="43" spans="1:17">
       <c r="A43" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="3" t="s">
@@ -2492,12 +2492,12 @@
     </row>
     <row r="44" spans="1:17">
       <c r="A44" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="D44" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -2513,9 +2513,9 @@
       </c>
       <c r="L44" s="8"/>
       <c r="M44" s="8"/>
-      <c r="N44" s="3"/>
+      <c r="N44" s="8"/>
       <c r="O44" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q44" t="s">
         <v>33</v>
@@ -2523,7 +2523,7 @@
     </row>
     <row r="45" spans="1:17">
       <c r="A45" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>43</v>
@@ -2551,12 +2551,12 @@
         <v>0</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:17">
       <c r="A46" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="3" t="s">
@@ -2576,12 +2576,12 @@
       </c>
       <c r="J46" s="9"/>
       <c r="O46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:17">
       <c r="A47" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -2597,7 +2597,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
       <c r="O47" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P47" s="1" t="s">
         <v>32</v>
@@ -2608,7 +2608,7 @@
     </row>
     <row r="48" spans="1:17">
       <c r="A48" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -2624,7 +2624,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
       <c r="O48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P48" s="1" t="s">
         <v>32</v>
@@ -2635,46 +2635,46 @@
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="J49" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="L49" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="M49" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="N49" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="O49" s="13" t="s">
         <v>112</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="I49" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="L49" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="M49" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="N49" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="O49" s="13" t="s">
-        <v>113</v>
       </c>
       <c r="P49" s="1" t="s">
         <v>32</v>
@@ -2688,7 +2688,7 @@
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>43</v>
@@ -2706,7 +2706,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
       <c r="O50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q50" t="s">
         <v>33</v>
@@ -2714,10 +2714,10 @@
     </row>
     <row r="51" spans="1:18">
       <c r="A51" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="14" t="s">
         <v>116</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>117</v>
       </c>
       <c r="C51" s="3"/>
       <c r="F51" s="3"/>
@@ -2728,37 +2728,37 @@
     </row>
     <row r="52" spans="1:18">
       <c r="A52" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="C52" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="O52" t="s">
         <v>119</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="O52" t="s">
-        <v>120</v>
       </c>
       <c r="Q52" t="s">
         <v>33</v>
@@ -2766,7 +2766,7 @@
     </row>
     <row r="53" spans="1:18">
       <c r="A53" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -2782,7 +2782,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="8"/>
       <c r="O53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P53" s="1" t="s">
         <v>32</v>
@@ -2793,7 +2793,7 @@
     </row>
     <row r="54" spans="1:18">
       <c r="A54" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
@@ -2808,7 +2808,7 @@
       <c r="M54" s="8"/>
       <c r="N54" s="8"/>
       <c r="O54" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P54" s="1" t="s">
         <v>32</v>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="55" spans="1:18">
       <c r="A55" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="3" t="s">
@@ -2845,7 +2845,7 @@
     </row>
     <row r="56" spans="1:18">
       <c r="A56" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -2861,7 +2861,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="8"/>
       <c r="O56" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P56" s="1" t="s">
         <v>32</v>
@@ -2872,7 +2872,7 @@
     </row>
     <row r="57" spans="1:18">
       <c r="A57" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>43</v>
@@ -2892,7 +2892,7 @@
       <c r="L57" s="8"/>
       <c r="M57" s="8"/>
       <c r="O57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P57" s="1" t="s">
         <v>32</v>
@@ -2903,7 +2903,7 @@
     </row>
     <row r="58" spans="1:18">
       <c r="A58" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>43</v>
@@ -2918,12 +2918,12 @@
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
       <c r="J58" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
       <c r="O58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P58" t="s">
         <v>73</v>
@@ -2934,7 +2934,7 @@
     </row>
     <row r="59" spans="1:18">
       <c r="A59" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>43</v>
@@ -2960,7 +2960,7 @@
         <v>48</v>
       </c>
       <c r="O59" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q59" t="s">
         <v>33</v>
@@ -2968,7 +2968,7 @@
     </row>
     <row r="60" spans="1:18">
       <c r="A60" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="3" t="s">
@@ -2996,12 +2996,12 @@
         <v>0</v>
       </c>
       <c r="O60" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:18">
       <c r="A61" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B61" s="8"/>
       <c r="C61">
@@ -3029,12 +3029,12 @@
         <v>0</v>
       </c>
       <c r="O61" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:18">
       <c r="A62" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -3055,7 +3055,7 @@
       <c r="M62" s="8"/>
       <c r="N62" s="8"/>
       <c r="O62" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P62" s="1" t="s">
         <v>32</v>
@@ -3066,7 +3066,7 @@
     </row>
     <row r="63" spans="1:18">
       <c r="A63" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
@@ -3086,7 +3086,7 @@
       <c r="L63" s="8"/>
       <c r="M63" s="8"/>
       <c r="O63" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P63" s="1" t="s">
         <v>32</v>
@@ -3097,7 +3097,7 @@
     </row>
     <row r="64" spans="1:18">
       <c r="A64" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -3121,12 +3121,12 @@
         <v>0</v>
       </c>
       <c r="O64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:17">
       <c r="A65" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B65" s="8"/>
       <c r="C65" s="3" t="s">
@@ -3152,12 +3152,12 @@
         <v>0</v>
       </c>
       <c r="O65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:17">
       <c r="A66" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B66" s="10" t="s">
         <v>43</v>
@@ -3179,7 +3179,7 @@
       <c r="L66" s="8"/>
       <c r="M66" s="8"/>
       <c r="O66" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P66" s="1" t="s">
         <v>32</v>
@@ -3190,7 +3190,7 @@
     </row>
     <row r="67" spans="1:17" ht="17" thickBot="1">
       <c r="A67" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B67" s="7">
         <f xml:space="preserve"> 66-8</f>
@@ -3225,20 +3225,20 @@
     </row>
     <row r="68" spans="1:17">
       <c r="Q68" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:17">
       <c r="A72" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:17">
       <c r="A73" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:17">
@@ -3246,7 +3246,7 @@
         <v>40</v>
       </c>
       <c r="B74" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:17">
@@ -3254,17 +3254,17 @@
         <v>67</v>
       </c>
       <c r="B75" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:17">
       <c r="B76" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:17">
       <c r="B77" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:17">
@@ -3272,39 +3272,39 @@
         <v>45</v>
       </c>
       <c r="B78" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:17">
       <c r="A79" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="80" spans="1:17">
       <c r="A80" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B80" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B81" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B82" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -3312,12 +3312,12 @@
         <v>42</v>
       </c>
       <c r="B83" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -3325,7 +3325,7 @@
         <v>42</v>
       </c>
       <c r="B89" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -3336,7 +3336,7 @@
         <v>55</v>
       </c>
       <c r="B91" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -3347,19 +3347,19 @@
         <v>59</v>
       </c>
       <c r="B93" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="15"/>
       <c r="B94" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="15"/>
       <c r="B95" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -3367,7 +3367,7 @@
         <v>64</v>
       </c>
       <c r="B97" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -3378,23 +3378,23 @@
         <v>71</v>
       </c>
       <c r="B99" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B101" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B103" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -3402,10 +3402,10 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B105" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D105" s="13"/>
     </row>
@@ -3414,10 +3414,10 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B107" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -3425,132 +3425,132 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B109" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D109" s="13"/>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B111" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="B113" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="B114" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="B115" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="B116" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="B117" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B119" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="B120" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="B121" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B123" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B125" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="B126" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B128" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="B129" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="B130" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="B131" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B133" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="B134" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="B135" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B137" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D137" s="13"/>
     </row>
@@ -3559,87 +3559,87 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B139" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B141" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="B142" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="B143" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="145" spans="1:5">
       <c r="A145" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B145" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="147" spans="1:5">
       <c r="A147" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B147" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="148" spans="1:5">
       <c r="B148" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="150" spans="1:5">
       <c r="A150" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B150" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B152" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B154" t="s">
         <v>14</v>
       </c>
       <c r="C154" t="s">
+        <v>192</v>
+      </c>
+      <c r="D154" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="D154" s="13" t="s">
+      <c r="E154" t="s">
         <v>194</v>
-      </c>
-      <c r="E154" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="155" spans="1:5">
       <c r="B155" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -3674,12 +3674,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -3714,67 +3714,67 @@
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -3785,7 +3785,7 @@
         <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -3796,7 +3796,7 @@
         <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -3807,7 +3807,7 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -3818,7 +3818,7 @@
         <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -3829,7 +3829,7 @@
         <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -3840,148 +3840,148 @@
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D34" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B36" t="s">
         <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B37" t="s">
         <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B38" t="s">
         <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D38" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B39" t="s">
         <v>32</v>
       </c>
       <c r="C39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B40" t="s">
         <v>32</v>
       </c>
       <c r="C40" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D40" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B41" t="s">
         <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B42" t="s">
         <v>32</v>
       </c>
       <c r="C42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B46" t="s">
         <v>32</v>
       </c>
       <c r="C46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3992,82 +3992,82 @@
         <v>32</v>
       </c>
       <c r="C47" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D47" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s">
         <v>32</v>
       </c>
       <c r="C48" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
         <v>32</v>
       </c>
       <c r="C49" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D49" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B50" t="s">
         <v>32</v>
       </c>
       <c r="C50" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B51" t="s">
         <v>32</v>
       </c>
       <c r="C51" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B52" t="s">
         <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B53" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C53" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>